<commit_message>
Added silica flour to the background GREET2023 file
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2023.xlsx
+++ b/Lookup table_prototyping_greet2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\oulongwen\projects\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED0BB77-1FA7-48F0-AE15-435841EA5691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB069AF-E2D7-4E93-90DE-36F75FF5E678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="5" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <definedName name="MT2T">[2]Fuel_Specs!$D$175</definedName>
     <definedName name="t2g">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5" concurrentManualCount="8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="388">
   <si>
     <t>Diesel</t>
   </si>
@@ -1494,6 +1494,18 @@
   </si>
   <si>
     <t>Need to adjust cell Catalyst!A5, results are in Catalyst!S134, etc. Unit conversion is needed.</t>
+  </si>
+  <si>
+    <t>Lignosulfonate</t>
+  </si>
+  <si>
+    <t>Silica flour</t>
+  </si>
+  <si>
+    <t>See the spreadsheet</t>
+  </si>
+  <si>
+    <t>See the pdf file, assuming 2.86 MJ of electricity per kg</t>
   </si>
 </sst>
 </file>
@@ -11584,11 +11596,11 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:CP29"/>
+  <dimension ref="A1:CR29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BY1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CB29" sqref="CB29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BS1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CR30" sqref="CR30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11602,7 +11614,7 @@
     <col min="32" max="32" width="22.42578125" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:96" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="10" t="s">
         <v>266</v>
@@ -11883,8 +11895,14 @@
       <c r="CP1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ1" t="s">
+        <v>384</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>338</v>
       </c>
@@ -12167,8 +12185,14 @@
       <c r="CP2" s="82" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ2" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="CR2" s="82" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -12451,8 +12475,14 @@
       <c r="CP3" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ3" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR3" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -12735,8 +12765,14 @@
       <c r="CP4" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ4" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR4" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -13019,8 +13055,14 @@
       <c r="CP5" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ5" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR5" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -13303,8 +13345,14 @@
       <c r="CP6" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ6" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR6" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -13587,8 +13635,14 @@
       <c r="CP7" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ7" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR7" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -13871,8 +13925,14 @@
       <c r="CP8" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ8" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR8" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>48</v>
       </c>
@@ -14155,8 +14215,14 @@
       <c r="CP9" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ9" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR9" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>49</v>
       </c>
@@ -14439,8 +14505,14 @@
       <c r="CP10" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ10" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR10" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>50</v>
       </c>
@@ -14723,8 +14795,14 @@
       <c r="CP11" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ11" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR11" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>51</v>
       </c>
@@ -15007,8 +15085,14 @@
       <c r="CP12" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ12" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR12" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>52</v>
       </c>
@@ -15291,8 +15375,14 @@
       <c r="CP13" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ13" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR13" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>53</v>
       </c>
@@ -15575,8 +15665,14 @@
       <c r="CP14" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ14" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR14" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>54</v>
       </c>
@@ -15859,8 +15955,14 @@
       <c r="CP15" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ15" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR15" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>55</v>
       </c>
@@ -16143,8 +16245,14 @@
       <c r="CP16" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ16" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR16" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>56</v>
       </c>
@@ -16427,8 +16535,14 @@
       <c r="CP17" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ17" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR17" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>57</v>
       </c>
@@ -16711,8 +16825,14 @@
       <c r="CP18" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ18" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR18" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>58</v>
       </c>
@@ -16995,8 +17115,14 @@
       <c r="CP19" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ19">
+        <v>0.18256971757000354</v>
+      </c>
+      <c r="CR19">
+        <v>0.34915976133752336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A20" s="78" t="s">
         <v>326</v>
       </c>
@@ -17279,8 +17405,14 @@
       <c r="CP20" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ20" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR20" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A21" s="78" t="s">
         <v>327</v>
       </c>
@@ -17563,8 +17695,14 @@
       <c r="CP21" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ21" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR21" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
         <v>328</v>
       </c>
@@ -17847,8 +17985,14 @@
       <c r="CP22" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ22" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR22" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A23" s="78" t="s">
         <v>329</v>
       </c>
@@ -18131,8 +18275,14 @@
       <c r="CP23" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ23" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR23" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A24" s="78" t="s">
         <v>330</v>
       </c>
@@ -18415,8 +18565,14 @@
       <c r="CP24" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ24" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR24" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A25" s="78" t="s">
         <v>331</v>
       </c>
@@ -18699,8 +18855,14 @@
       <c r="CP25" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ25" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR25" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A26" s="78" t="s">
         <v>332</v>
       </c>
@@ -18983,8 +19145,14 @@
       <c r="CP26" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ26" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR26" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A27" s="79" t="s">
         <v>333</v>
       </c>
@@ -19267,12 +19435,18 @@
       <c r="CP27" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="CQ27" s="109">
+        <v>0</v>
+      </c>
+      <c r="CR27" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:96" x14ac:dyDescent="0.25">
       <c r="AI28" s="75"/>
       <c r="AK28" s="75"/>
     </row>
-    <row r="29" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -19420,6 +19594,12 @@
       <c r="CI29" s="134"/>
       <c r="CJ29" s="134"/>
       <c r="CK29" s="134"/>
+      <c r="CQ29" t="s">
+        <v>386</v>
+      </c>
+      <c r="CR29" t="s">
+        <v>387</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -20524,7 +20704,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>

</xml_diff>